<commit_message>
Show category/subcategory names in Excel template dropdowns
- Update CategoryLookup and SubcategoryLookup sheets to show 'Name (code)' format
- Users see readable names like 'Income (income)' instead of just codes
- Update parser to extract code from parentheses if present
- Maintains backward compatibility with code-only format

Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/backend/static/Monytix_Statement_Template.xlsx
+++ b/backend/static/Monytix_Statement_Template.xlsx
@@ -427,196 +427,196 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>category_code</t>
+          <t>category_display</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>income</t>
+          <t>Income (income)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>transfers_in</t>
+          <t>Transfers In (transfers_in)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>transfers_out</t>
+          <t>Transfers Out (transfers_out)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>loans_payments</t>
+          <t>Loan Payments (EMIs) (loans_payments)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>investments_commitments</t>
+          <t>Regular Investments / Commitments (investments_commitments)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>insurance_premiums</t>
+          <t>Insurance Premiums (insurance_premiums)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>housing_fixed</t>
+          <t>Housing (Rent &amp; Society) (housing_fixed)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>utilities</t>
+          <t>Utilities (utilities)</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment &amp; OTT (entertainment)</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>food_dining</t>
+          <t>Food &amp; Dining / Nightlife (food_dining)</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>groceries</t>
+          <t>Groceries (groceries)</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>medical</t>
+          <t>Medical &amp; Healthcare (medical)</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>fitness</t>
+          <t>Fitness &amp; Sports (fitness)</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>transport</t>
+          <t>Transport &amp; Travel (transport)</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>shopping</t>
+          <t>Shopping &amp; Retail (shopping)</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>Education (education)</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>child_care</t>
+          <t>Child Care (child_care)</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>motor_maintenance</t>
+          <t>Motor Maintenance (motor_maintenance)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>pets</t>
+          <t>Pets (pets)</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>banks</t>
+          <t>Bank Interest &amp; Fees (banks)</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>govt_tax</t>
+          <t>Government Taxes (govt_tax)</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>charity_donations</t>
+          <t>Charity &amp; Donations (charity_donations)</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>festivals_rituals</t>
+          <t>Festivals, Rituals &amp; Celebrations (festivals_rituals)</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>family_support</t>
+          <t>Family Support &amp; Obligations (family_support)</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>business_expenses</t>
+          <t>Business &amp; Freelance Expenses (business_expenses)</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>govt_benefits</t>
+          <t>Government Benefits &amp; Subsidies (govt_benefits)</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>credit_cards</t>
+          <t>Credit Cards (credit_cards)</t>
         </is>
       </c>
     </row>
@@ -642,1141 +642,1141 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>subcategory_code</t>
+          <t>subcategory_display</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>amazon</t>
+          <t>Online Shopping (amazon)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>bank_charges</t>
+          <t>Bank Charges / Fees (bank_charges)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>bank_interest</t>
+          <t>Interest Credit (Bank) (bank_interest)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>bank_sweep</t>
+          <t>Savings Sweep / Auto (bank_sweep)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>biz_marketing</t>
+          <t>Ads, Marketing, Campaigns (biz_marketing)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>biz_other</t>
+          <t>Other Business Expenses (biz_other)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>biz_raw_materials</t>
+          <t>Materials / Inventory (biz_raw_materials)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>biz_rent</t>
+          <t>Office / Shop Rent (biz_rent)</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>biz_salary</t>
+          <t>Salaries/Stipends to Staff (biz_salary)</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>biz_tools_software</t>
+          <t>Tools, SaaS, Domains, Hosting (biz_tools_software)</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>biz_travel</t>
+          <t>Client Travel &amp; Stays (biz_travel)</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>cc_balance_transfer</t>
+          <t>Credit Card Balance Transfer (cc_balance_transfer)</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>cc_bill_payment</t>
+          <t>Credit Card Bill Payment (cc_bill_payment)</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>cc_cashback</t>
+          <t>Credit Card Cashback / Rewards (Income) (cc_cashback)</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>cc_emi</t>
+          <t>Credit Card EMI / Installments (cc_emi)</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>cc_fees</t>
+          <t>Credit Card Fees (Annual/Late/Overlimit) (cc_fees)</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>cc_foreign_transaction</t>
+          <t>Foreign Transaction Fee (cc_foreign_transaction)</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>cc_interest</t>
+          <t>Credit Card Interest / Finance Charges (cc_interest)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>cc_other</t>
+          <t>Other Credit Card Charges (cc_other)</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>char_church</t>
+          <t>Church Offerings (char_church)</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>char_crowdfund</t>
+          <t>Crowdfunding / Medical Help (char_crowdfund)</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>char_gurudwara</t>
+          <t>Gurudwara / Langar / Seva (char_gurudwara)</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>char_mosque</t>
+          <t>Mosque / Zakat / Sadaqah (char_mosque)</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>char_ngo</t>
+          <t>NGOs &amp; Social Causes (char_ngo)</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>char_other</t>
+          <t>Other Donations &amp; Offerings (char_other)</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>char_temple</t>
+          <t>Temple / Puja / Hundi (char_temple)</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>child_daycare</t>
+          <t>Daycare / Babysitting (child_daycare)</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>child_education</t>
+          <t>Child Education Expenses (child_education)</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>edu_online</t>
+          <t>Online Courses / Certifications (edu_online)</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>edu_school_fees</t>
+          <t>School / College Fees (edu_school_fees)</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>edu_tuition</t>
+          <t>Tuition / Coaching (edu_tuition)</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>electricity</t>
+          <t>Electricity Bill (electricity)</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>ent_adventure</t>
+          <t>Adventure &amp; Recreation (ent_adventure)</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>ent_amusement</t>
+          <t>Amusement Parks &amp; Events (ent_amusement)</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>ent_casinos</t>
+          <t>Casinos &amp; Gambling (ent_casinos)</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>ent_cultural</t>
+          <t>Cultural &amp; Festive Events (ent_cultural)</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>ent_gaming</t>
+          <t>Video Games &amp; eSports (ent_gaming)</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>ent_movies_ott</t>
+          <t>Movies &amp; TV / OTT (ent_movies_ott)</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>ent_museums_arts</t>
+          <t>Museums &amp; Art Exhibitions (ent_museums_arts)</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>ent_music</t>
+          <t>Music &amp; Audio (ent_music)</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>ent_nightlife</t>
+          <t>Nightlife &amp; Parties (ent_nightlife)</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>ent_other</t>
+          <t>Other Entertainment (ent_other)</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ent_sports_events</t>
+          <t>Sporting Events &amp; Tickets (ent_sports_events)</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>fam_education_help</t>
+          <t>Paying Relatives' Education Fees (fam_education_help)</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>fam_medical_help</t>
+          <t>Helping Family with Medical Bills (fam_medical_help)</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>fam_other</t>
+          <t>Other Family Support (fam_other)</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>fam_parents</t>
+          <t>Monthly Support to Parents/In-laws (fam_parents)</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>fam_relatives</t>
+          <t>Support to Siblings/Relatives (fam_relatives)</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>fd_cafes</t>
+          <t>Cafés &amp; Bakeries (fd_cafes)</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>fd_desserts</t>
+          <t>Desserts &amp; Sweet Shops (fd_desserts)</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>fd_fine</t>
+          <t>Fine &amp; Casual Dining (fd_fine)</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>fd_online</t>
+          <t>Online Food Delivery (Swiggy/Zomato) (fd_online)</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>fd_pan_shop</t>
+          <t>Pan / Cigarette Shop (fd_pan_shop)</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>fd_pubs_bars</t>
+          <t>Pubs &amp; Bars (fd_pubs_bars)</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>fd_quick_service</t>
+          <t>Quick Service / Fast Food (fd_quick_service)</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>fd_street_food</t>
+          <t>Street Food &amp; Local Eateries (fd_street_food)</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>fest_clothing</t>
+          <t>Festival Clothing &amp; Wear (fest_clothing)</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>fest_decor</t>
+          <t>Decorations &amp; Lights (fest_decor)</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>fest_gifts</t>
+          <t>Festival Gifts (fest_gifts)</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>fest_other</t>
+          <t>Other Festival Expenses (fest_other)</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>fest_pandal</t>
+          <t>Pandal / Mandap &amp; Events (fest_pandal)</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>fest_pooja_items</t>
+          <t>Puja Items &amp; Ritual Needs (fest_pooja_items)</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>fest_sweets</t>
+          <t>Sweets &amp; Snacks (fest_sweets)</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>fit_gyms</t>
+          <t>Gyms &amp; Fitness Centers (fit_gyms)</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>fit_sports</t>
+          <t>Sports &amp; Coaching / Gear (fit_sports)</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>flight</t>
+          <t>Flights (flight)</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>govt_other_benefits</t>
+          <t>Other Government Benefits (govt_other_benefits)</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>govt_scheme</t>
+          <t>PM Kisan, Pensions, Welfare Schemes (govt_scheme)</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>govt_subsidy</t>
+          <t>LPG, Fertilizer &amp; Other Subsidies (govt_subsidy)</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>groc_fv</t>
+          <t>Vegetable &amp; Fruit Stores (groc_fv)</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>groc_hyper</t>
+          <t>Hypermarkets / Department Stores (groc_hyper)</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>groc_meat</t>
+          <t>Meat / Poultry / Seafood (groc_meat)</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>groc_online</t>
+          <t>Online Groceries / Q-commerce (groc_online)</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>house_maid</t>
+          <t>Maid / Security / House Help (house_maid)</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>house_rent</t>
+          <t>Rent (house_rent)</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>house_society</t>
+          <t>Society / Maintenance (house_society)</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>inc_business</t>
+          <t>Business Income (inc_business)</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>inc_dividend</t>
+          <t>Dividends (inc_dividend)</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>inc_interest</t>
+          <t>Interest Income (inc_interest)</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>inc_other</t>
+          <t>Other Income (inc_other)</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>inc_salary</t>
+          <t>Salary / Payroll (inc_salary)</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>inc_side</t>
+          <t>Side Income / Freelance (inc_side)</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>inc_tax_refund</t>
+          <t>Tax Refund (inc_tax_refund)</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>ins_health</t>
+          <t>Health Insurance (ins_health)</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>ins_home_other</t>
+          <t>Home / Other Insurance (ins_home_other)</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>ins_life</t>
+          <t>Life Insurance (ins_life)</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>ins_motor</t>
+          <t>Motor Insurance (ins_motor)</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>inv_fd_rd</t>
+          <t>FD / RD (inv_fd_rd)</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>inv_gold</t>
+          <t>Gold / SGB (inv_gold)</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>inv_nps</t>
+          <t>NPS (inv_nps)</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>inv_ppf</t>
+          <t>PPF (inv_ppf)</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>inv_sip</t>
+          <t>Mutual Fund SIP (inv_sip)</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>inv_stocks</t>
+          <t>Stocks / ETFs (inv_stocks)</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>loan_bike</t>
+          <t>Two-Wheeler EMI (loan_bike)</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>loan_car</t>
+          <t>Car Loan EMI (loan_car)</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>loan_cc_bill</t>
+          <t>Credit Card Bill Payment (loan_cc_bill)</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>loan_home</t>
+          <t>Home Loan EMI (loan_home)</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>loan_other</t>
+          <t>Other Loan/Debt Payment (loan_other)</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>loan_personal</t>
+          <t>Personal Loan EMI (loan_personal)</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>loan_student</t>
+          <t>Education Loan EMI (loan_student)</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>med_apps</t>
+          <t>Medical Apps / Services (med_apps)</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>med_dental</t>
+          <t>Dental Care (med_dental)</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>med_eye</t>
+          <t>Eye Care / Optometry (med_eye)</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>med_general</t>
+          <t>General / Hospitals / Nursing (med_general)</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>med_other</t>
+          <t>Other Medical (med_other)</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>med_pharma</t>
+          <t>Pharmacies &amp; Supplements (med_pharma)</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>mobile</t>
+          <t>Mobile/Internet (mobile)</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>motor_insurance</t>
+          <t>Motor Insurance (motor_insurance)</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>motor_services</t>
+          <t>General Services / Repairs (motor_services)</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>pet_food</t>
+          <t>Pet Food (pet_food)</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>pet_grooming</t>
+          <t>Grooming / Boarding / Bathing (pet_grooming)</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>pet_insurance</t>
+          <t>Pet Insurance (pet_insurance)</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>pet_vaccine</t>
+          <t>Vaccination / Vet (pet_vaccine)</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>recurring_deposit</t>
+          <t>Recurring Deposit (recurring_deposit)</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>restaurant</t>
+          <t>Restaurant (restaurant)</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>shop_auto_supplies</t>
+          <t>Automotive Supplies (shop_auto_supplies)</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>shop_beauty</t>
+          <t>Beauty &amp; Personal Care (shop_beauty)</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>shop_books_media</t>
+          <t>Books &amp; Media (shop_books_media)</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>shop_children_toys</t>
+          <t>Children &amp; Toys (shop_children_toys)</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>shop_clothing</t>
+          <t>Clothing &amp; Accessories (shop_clothing)</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>shop_electronics</t>
+          <t>Electronics &amp; Gadgets (shop_electronics)</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>shop_general</t>
+          <t>General Merchandise (shop_general)</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>shop_gifts</t>
+          <t>Gifts &amp; Novelties (shop_gifts)</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>shop_hobbies</t>
+          <t>Hobbies &amp; Crafts (shop_hobbies)</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>shop_home_kitchen</t>
+          <t>Home &amp; Kitchen / Furnishings (shop_home_kitchen)</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>shop_marketplaces</t>
+          <t>Online Marketplaces (shop_marketplaces)</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>shop_pet_supplies</t>
+          <t>Pet Supplies (shop_pet_supplies)</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>shop_sports_outdoor</t>
+          <t>Sports &amp; Outdoor (shop_sports_outdoor)</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>shop_stationery</t>
+          <t>Stationery &amp; Office Supplies (shop_stationery)</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>supermarket</t>
+          <t>Supermarket (supermarket)</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>tax_gst</t>
+          <t>GST / Challan (tax_gst)</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>tax_income</t>
+          <t>Income Tax / TDS (tax_income)</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>tax_other</t>
+          <t>Other Government Taxes (tax_other)</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>tr_apps</t>
+          <t>Transport Apps (Uber/Ola etc.) (tr_apps)</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>tr_fuel</t>
+          <t>Fuel / Petrol / Diesel (tr_fuel)</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>tr_in_deposit</t>
+          <t>Cash/Cheque/ATM Deposit (tr_in_deposit)</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>tr_in_internal</t>
+          <t>Account Transfer In (tr_in_internal)</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>tr_in_invest_ret</t>
+          <t>From Investments / PF / Retirement (tr_in_invest_ret)</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>tr_in_other</t>
+          <t>Other Transfer In (tr_in_other)</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>tr_in_savings</t>
+          <t>Savings Sweep / Sweep In (tr_in_savings)</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>tr_lodging</t>
+          <t>Hotels / Stays / Airbnb (tr_lodging)</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>tr_other</t>
+          <t>Other Transport (tr_other)</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>tr_out_atm</t>
+          <t>Cash / ATM Withdrawal (tr_out_atm)</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>tr_out_other</t>
+          <t>Other Transfer Out (tr_out_other)</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>tr_out_savings</t>
+          <t>Transfer to Savings/Joint (tr_out_savings)</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>tr_out_sweep</t>
+          <t>Sweep Out (FD / Linked) (tr_out_sweep)</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>tr_out_wallet</t>
+          <t>Bank → Wallet / UPI (tr_out_wallet)</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>tr_public</t>
+          <t>Public Transit (Rail/Metro/Bus) (tr_public)</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>tr_taxis</t>
+          <t>Taxis / Auto / Ride-share (tr_taxis)</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>tr_tolls</t>
+          <t>Tolls / FASTag (tr_tolls)</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>tr_travel</t>
+          <t>Flights / Bus / Train / Cruise (tr_travel)</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>uber</t>
+          <t>Cabs (uber)</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>util_broadband</t>
+          <t>Internet / Broadband (util_broadband)</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>util_dth_cable</t>
+          <t>DTH / Cable TV (util_dth_cable)</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>util_electricity</t>
+          <t>Electricity (util_electricity)</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>util_gas_lpg</t>
+          <t>Gas / LPG / PNG (util_gas_lpg)</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>util_mobile</t>
+          <t>Mobile / Telephone (util_mobile)</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>util_other</t>
+          <t>Other Utilities (util_other)</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>util_sewage_waste</t>
+          <t>Sewage / Waste Mgmt (util_sewage_waste)</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>util_water</t>
+          <t>Water (util_water)</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>water</t>
+          <t>Water Bill (water)</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>zomato</t>
+          <t>Food Delivery (zomato)</t>
         </is>
       </c>
     </row>

</xml_diff>